<commit_message>
CPU symbol changed, all pins on one page
</commit_message>
<xml_diff>
--- a/SAME70_Pins.xlsx
+++ b/SAME70_Pins.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa4fa29a32d88222/PROJEKTE/ATSAME70/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/aa4fa29a32d88222/PROJEKTE/TelescopeDriver25/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="486" documentId="8_{FAEC4C7A-5A7E-4F8B-ADAA-0E58951849F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3631FCEA-D5E2-4E2B-85E2-127D2387403B}"/>
+  <xr:revisionPtr revIDLastSave="490" documentId="8_{FAEC4C7A-5A7E-4F8B-ADAA-0E58951849F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{129EB731-D999-45FF-940A-F2DD526F1768}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="27288" windowHeight="17544" xr2:uid="{63881150-7A5B-4E3D-8F91-5A59AC3825CF}"/>
   </bookViews>
@@ -3938,7 +3938,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -4116,6 +4116,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20 % - Akzent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -4172,10 +4175,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4495,12 +4494,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3941833B-CC47-4797-9275-893CD4E748EC}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:AA181"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G46" sqref="G46"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4641,7 +4639,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A3" s="19">
         <v>1</v>
       </c>
@@ -4703,7 +4701,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A4" s="19">
         <v>2</v>
       </c>
@@ -4765,7 +4763,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A5" s="19">
         <v>3</v>
       </c>
@@ -4833,7 +4831,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A6" s="19">
         <v>4</v>
       </c>
@@ -4901,7 +4899,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="7" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A7" s="19">
         <v>5</v>
       </c>
@@ -4969,7 +4967,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="8" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A8" s="19">
         <v>6</v>
       </c>
@@ -5037,7 +5035,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A9" s="19">
         <v>7</v>
       </c>
@@ -5099,7 +5097,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="10" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A10" s="19">
         <v>8</v>
       </c>
@@ -5167,7 +5165,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="11" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A11" s="19">
         <v>9</v>
       </c>
@@ -5235,7 +5233,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A12" s="19">
         <v>10</v>
       </c>
@@ -5303,7 +5301,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="13" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A13" s="19">
         <v>11</v>
       </c>
@@ -5371,7 +5369,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="14" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A14" s="19">
         <v>12</v>
       </c>
@@ -5439,7 +5437,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="15" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A15" s="19">
         <v>13</v>
       </c>
@@ -5507,7 +5505,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="16" spans="1:27" hidden="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A16" s="19">
         <v>14</v>
       </c>
@@ -5575,7 +5573,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="17" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A17" s="19">
         <v>15</v>
       </c>
@@ -5643,7 +5641,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="18" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A18" s="19">
         <v>16</v>
       </c>
@@ -5705,7 +5703,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="19" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A19" s="19">
         <v>17</v>
       </c>
@@ -5767,7 +5765,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="20" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A20" s="19">
         <v>18</v>
       </c>
@@ -5835,7 +5833,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="21" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A21" s="19">
         <v>19</v>
       </c>
@@ -5903,7 +5901,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="22" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A22" s="19">
         <v>20</v>
       </c>
@@ -5971,7 +5969,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="23" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A23" s="19">
         <v>21</v>
       </c>
@@ -6039,7 +6037,7 @@
         <v>198</v>
       </c>
     </row>
-    <row r="24" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A24" s="19">
         <v>22</v>
       </c>
@@ -6107,7 +6105,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="25" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A25" s="19">
         <v>23</v>
       </c>
@@ -6175,7 +6173,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="26" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A26" s="19">
         <v>24</v>
       </c>
@@ -6243,7 +6241,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="27" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A27" s="19">
         <v>25</v>
       </c>
@@ -6311,7 +6309,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="28" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A28" s="19">
         <v>26</v>
       </c>
@@ -6376,7 +6374,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="29" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A29" s="19">
         <v>27</v>
       </c>
@@ -6441,7 +6439,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="30" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A30" s="19">
         <v>28</v>
       </c>
@@ -6506,7 +6504,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="31" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A31" s="19">
         <v>29</v>
       </c>
@@ -6571,7 +6569,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="32" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A32" s="19">
         <v>30</v>
       </c>
@@ -6633,7 +6631,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="33" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A33" s="19">
         <v>31</v>
       </c>
@@ -6698,7 +6696,7 @@
         <v>237</v>
       </c>
     </row>
-    <row r="34" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A34" s="19">
         <v>32</v>
       </c>
@@ -7573,11 +7571,11 @@
         <v>362</v>
       </c>
     </row>
-    <row r="47" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A47" s="19">
         <v>45</v>
       </c>
-      <c r="B47" s="56" t="s">
+      <c r="B47" s="69" t="s">
         <v>363</v>
       </c>
       <c r="C47" s="19" t="s">
@@ -7635,11 +7633,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A48" s="19">
         <v>46</v>
       </c>
-      <c r="B48" s="56" t="s">
+      <c r="B48" s="69" t="s">
         <v>369</v>
       </c>
       <c r="C48" s="19" t="s">
@@ -7697,11 +7695,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="49" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A49" s="19">
         <v>47</v>
       </c>
-      <c r="B49" s="56" t="s">
+      <c r="B49" s="69" t="s">
         <v>372</v>
       </c>
       <c r="C49" s="19" t="s">
@@ -7759,11 +7757,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="50" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A50" s="19">
         <v>48</v>
       </c>
-      <c r="B50" s="56" t="s">
+      <c r="B50" s="69" t="s">
         <v>377</v>
       </c>
       <c r="C50" s="19" t="s">
@@ -7821,11 +7819,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="51" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A51" s="19">
         <v>49</v>
       </c>
-      <c r="B51" s="56" t="s">
+      <c r="B51" s="69" t="s">
         <v>382</v>
       </c>
       <c r="C51" s="19" t="s">
@@ -7883,11 +7881,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="52" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A52" s="19">
         <v>50</v>
       </c>
-      <c r="B52" s="56" t="s">
+      <c r="B52" s="69" t="s">
         <v>386</v>
       </c>
       <c r="C52" s="19" t="s">
@@ -7945,11 +7943,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="53" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A53" s="19">
         <v>51</v>
       </c>
-      <c r="B53" s="56" t="s">
+      <c r="B53" s="69" t="s">
         <v>391</v>
       </c>
       <c r="C53" s="19" t="s">
@@ -8007,11 +8005,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="54" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A54" s="19">
         <v>52</v>
       </c>
-      <c r="B54" s="56" t="s">
+      <c r="B54" s="69" t="s">
         <v>396</v>
       </c>
       <c r="C54" s="19" t="s">
@@ -8069,11 +8067,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="55" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A55" s="19">
         <v>53</v>
       </c>
-      <c r="B55" s="56" t="s">
+      <c r="B55" s="69" t="s">
         <v>400</v>
       </c>
       <c r="C55" s="19" t="s">
@@ -8131,11 +8129,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="56" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A56" s="19">
         <v>54</v>
       </c>
-      <c r="B56" s="56" t="s">
+      <c r="B56" s="69" t="s">
         <v>405</v>
       </c>
       <c r="C56" s="19" t="s">
@@ -8193,11 +8191,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="57" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A57" s="19">
         <v>55</v>
       </c>
-      <c r="B57" s="56" t="s">
+      <c r="B57" s="69" t="s">
         <v>409</v>
       </c>
       <c r="C57" s="19" t="s">
@@ -8255,11 +8253,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A58" s="19">
         <v>56</v>
       </c>
-      <c r="B58" s="56" t="s">
+      <c r="B58" s="69" t="s">
         <v>415</v>
       </c>
       <c r="C58" s="19" t="s">
@@ -8317,11 +8315,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="59" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A59" s="19">
         <v>57</v>
       </c>
-      <c r="B59" s="56" t="s">
+      <c r="B59" s="69" t="s">
         <v>420</v>
       </c>
       <c r="C59" s="19" t="s">
@@ -8379,11 +8377,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="60" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A60" s="19">
         <v>58</v>
       </c>
-      <c r="B60" s="56" t="s">
+      <c r="B60" s="69" t="s">
         <v>428</v>
       </c>
       <c r="C60" s="19" t="s">
@@ -8441,11 +8439,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="61" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A61" s="19">
         <v>59</v>
       </c>
-      <c r="B61" s="56" t="s">
+      <c r="B61" s="69" t="s">
         <v>432</v>
       </c>
       <c r="C61" s="19" t="s">
@@ -8503,11 +8501,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="62" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A62" s="19">
         <v>60</v>
       </c>
-      <c r="B62" s="56" t="s">
+      <c r="B62" s="69" t="s">
         <v>438</v>
       </c>
       <c r="C62" s="19" t="s">
@@ -8565,11 +8563,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="63" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A63" s="19">
         <v>61</v>
       </c>
-      <c r="B63" s="56" t="s">
+      <c r="B63" s="69" t="s">
         <v>442</v>
       </c>
       <c r="C63" s="19" t="s">
@@ -8627,11 +8625,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="64" spans="1:20" hidden="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A64" s="19">
         <v>62</v>
       </c>
-      <c r="B64" s="56" t="s">
+      <c r="B64" s="69" t="s">
         <v>445</v>
       </c>
       <c r="C64" s="19" t="s">
@@ -8689,11 +8687,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="65" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A65" s="19">
         <v>63</v>
       </c>
-      <c r="B65" s="56" t="s">
+      <c r="B65" s="69" t="s">
         <v>448</v>
       </c>
       <c r="C65" s="19" t="s">
@@ -8751,11 +8749,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="66" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A66" s="19">
         <v>64</v>
       </c>
-      <c r="B66" s="56" t="s">
+      <c r="B66" s="69" t="s">
         <v>451</v>
       </c>
       <c r="C66" s="19" t="s">
@@ -8813,11 +8811,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="67" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A67" s="19">
         <v>65</v>
       </c>
-      <c r="B67" s="56" t="s">
+      <c r="B67" s="69" t="s">
         <v>454</v>
       </c>
       <c r="C67" s="19" t="s">
@@ -8875,11 +8873,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="68" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A68" s="19">
         <v>66</v>
       </c>
-      <c r="B68" s="56" t="s">
+      <c r="B68" s="69" t="s">
         <v>457</v>
       </c>
       <c r="C68" s="19" t="s">
@@ -8937,11 +8935,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="69" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A69" s="19">
         <v>67</v>
       </c>
-      <c r="B69" s="56" t="s">
+      <c r="B69" s="69" t="s">
         <v>459</v>
       </c>
       <c r="C69" s="19" t="s">
@@ -8999,11 +8997,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="70" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A70" s="19">
         <v>68</v>
       </c>
-      <c r="B70" s="56" t="s">
+      <c r="B70" s="69" t="s">
         <v>464</v>
       </c>
       <c r="C70" s="19" t="s">
@@ -9061,11 +9059,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="71" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A71" s="19">
         <v>69</v>
       </c>
-      <c r="B71" s="56" t="s">
+      <c r="B71" s="69" t="s">
         <v>469</v>
       </c>
       <c r="C71" s="19" t="s">
@@ -9123,11 +9121,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="72" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A72" s="19">
         <v>70</v>
       </c>
-      <c r="B72" s="56" t="s">
+      <c r="B72" s="69" t="s">
         <v>474</v>
       </c>
       <c r="C72" s="19" t="s">
@@ -9185,11 +9183,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="73" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A73" s="19">
         <v>71</v>
       </c>
-      <c r="B73" s="56" t="s">
+      <c r="B73" s="69" t="s">
         <v>479</v>
       </c>
       <c r="C73" s="19" t="s">
@@ -9247,11 +9245,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="74" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A74" s="19">
         <v>72</v>
       </c>
-      <c r="B74" s="56" t="s">
+      <c r="B74" s="69" t="s">
         <v>484</v>
       </c>
       <c r="C74" s="19" t="s">
@@ -9309,11 +9307,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="75" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A75" s="19">
         <v>73</v>
       </c>
-      <c r="B75" s="56" t="s">
+      <c r="B75" s="69" t="s">
         <v>491</v>
       </c>
       <c r="C75" s="19" t="s">
@@ -9371,11 +9369,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="76" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A76" s="19">
         <v>74</v>
       </c>
-      <c r="B76" s="56" t="s">
+      <c r="B76" s="69" t="s">
         <v>496</v>
       </c>
       <c r="C76" s="19" t="s">
@@ -9433,11 +9431,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="77" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A77" s="19">
         <v>75</v>
       </c>
-      <c r="B77" s="56" t="s">
+      <c r="B77" s="69" t="s">
         <v>501</v>
       </c>
       <c r="C77" s="19" t="s">
@@ -9495,11 +9493,11 @@
         <v>32</v>
       </c>
     </row>
-    <row r="78" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A78" s="19">
         <v>76</v>
       </c>
-      <c r="B78" s="56" t="s">
+      <c r="B78" s="69" t="s">
         <v>507</v>
       </c>
       <c r="C78" s="19" t="s">
@@ -9557,7 +9555,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="79" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A79" s="19">
         <v>77</v>
       </c>
@@ -9625,7 +9623,7 @@
         <v>521</v>
       </c>
     </row>
-    <row r="80" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A80" s="19">
         <v>78</v>
       </c>
@@ -9693,7 +9691,7 @@
         <v>527</v>
       </c>
     </row>
-    <row r="81" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A81" s="19">
         <v>79</v>
       </c>
@@ -9761,7 +9759,7 @@
         <v>532</v>
       </c>
     </row>
-    <row r="82" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A82" s="19">
         <v>80</v>
       </c>
@@ -9829,7 +9827,7 @@
         <v>539</v>
       </c>
     </row>
-    <row r="83" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A83" s="19">
         <v>81</v>
       </c>
@@ -9897,7 +9895,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="84" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A84" s="19">
         <v>82</v>
       </c>
@@ -9965,7 +9963,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="85" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A85" s="19">
         <v>83</v>
       </c>
@@ -10033,7 +10031,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="86" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A86" s="19">
         <v>84</v>
       </c>
@@ -10101,7 +10099,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="87" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A87" s="19">
         <v>85</v>
       </c>
@@ -10169,7 +10167,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="88" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A88" s="19">
         <v>86</v>
       </c>
@@ -10237,7 +10235,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="89" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A89" s="19">
         <v>87</v>
       </c>
@@ -10305,7 +10303,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="90" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A90" s="19">
         <v>88</v>
       </c>
@@ -10373,7 +10371,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="91" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A91" s="19">
         <v>89</v>
       </c>
@@ -10441,7 +10439,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="92" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A92" s="19">
         <v>90</v>
       </c>
@@ -10509,7 +10507,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="93" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A93" s="19">
         <v>91</v>
       </c>
@@ -10577,7 +10575,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="94" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A94" s="19">
         <v>92</v>
       </c>
@@ -10645,7 +10643,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="95" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A95" s="19">
         <v>93</v>
       </c>
@@ -10713,7 +10711,7 @@
         <v>622</v>
       </c>
     </row>
-    <row r="96" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A96" s="19">
         <v>94</v>
       </c>
@@ -10781,7 +10779,7 @@
         <v>628</v>
       </c>
     </row>
-    <row r="97" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A97" s="19">
         <v>95</v>
       </c>
@@ -10849,7 +10847,7 @@
         <v>633</v>
       </c>
     </row>
-    <row r="98" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A98" s="19">
         <v>96</v>
       </c>
@@ -10917,7 +10915,7 @@
         <v>637</v>
       </c>
     </row>
-    <row r="99" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A99" s="19">
         <v>97</v>
       </c>
@@ -10985,7 +10983,7 @@
         <v>642</v>
       </c>
     </row>
-    <row r="100" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A100" s="19">
         <v>98</v>
       </c>
@@ -11053,7 +11051,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="101" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A101" s="19">
         <v>99</v>
       </c>
@@ -11121,7 +11119,7 @@
         <v>656</v>
       </c>
     </row>
-    <row r="102" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A102" s="19">
         <v>100</v>
       </c>
@@ -11183,7 +11181,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="103" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A103" s="19">
         <v>101</v>
       </c>
@@ -11248,7 +11246,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="104" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A104" s="19">
         <v>102</v>
       </c>
@@ -11316,7 +11314,7 @@
         <v>673</v>
       </c>
     </row>
-    <row r="105" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A105" s="19">
         <v>103</v>
       </c>
@@ -11384,7 +11382,7 @@
         <v>677</v>
       </c>
     </row>
-    <row r="106" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A106" s="19">
         <v>104</v>
       </c>
@@ -11452,7 +11450,7 @@
         <v>684</v>
       </c>
     </row>
-    <row r="107" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A107" s="19">
         <v>105</v>
       </c>
@@ -11514,7 +11512,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="108" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A108" s="19">
         <v>106</v>
       </c>
@@ -11576,7 +11574,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="109" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A109" s="19">
         <v>107</v>
       </c>
@@ -11638,7 +11636,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="110" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A110" s="19">
         <v>108</v>
       </c>
@@ -11706,7 +11704,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="111" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A111" s="19">
         <v>109</v>
       </c>
@@ -11768,7 +11766,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="112" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A112" s="19">
         <v>110</v>
       </c>
@@ -11830,7 +11828,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="113" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A113" s="19">
         <v>111</v>
       </c>
@@ -11892,7 +11890,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="114" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A114" s="19">
         <v>112</v>
       </c>
@@ -11954,7 +11952,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="115" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A115" s="19">
         <v>113</v>
       </c>
@@ -12016,7 +12014,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="116" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A116" s="19">
         <v>114</v>
       </c>
@@ -12078,7 +12076,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="117" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B117" s="56" t="s">
         <v>906</v>
       </c>
@@ -12137,7 +12135,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="118" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B118" s="56" t="s">
         <v>907</v>
       </c>
@@ -12196,7 +12194,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="119" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B119" s="56" t="s">
         <v>908</v>
       </c>
@@ -12255,7 +12253,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="120" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B120" s="56" t="s">
         <v>909</v>
       </c>
@@ -12314,7 +12312,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="121" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B121" s="56" t="s">
         <v>910</v>
       </c>
@@ -12373,7 +12371,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="122" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B122" s="56" t="s">
         <v>911</v>
       </c>
@@ -12432,7 +12430,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="123" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B123" s="56" t="s">
         <v>49</v>
       </c>
@@ -12491,7 +12489,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="124" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B124" s="56" t="s">
         <v>49</v>
       </c>
@@ -12550,7 +12548,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="125" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B125" s="56" t="s">
         <v>49</v>
       </c>
@@ -12609,7 +12607,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="126" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B126" s="56" t="s">
         <v>49</v>
       </c>
@@ -12668,7 +12666,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="127" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B127" s="56" t="s">
         <v>745</v>
       </c>
@@ -12733,7 +12731,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="128" spans="1:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:26" x14ac:dyDescent="0.3">
       <c r="B128" s="56" t="s">
         <v>751</v>
       </c>
@@ -12798,7 +12796,7 @@
         <v>753</v>
       </c>
     </row>
-    <row r="129" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B129" s="56" t="s">
         <v>754</v>
       </c>
@@ -12857,7 +12855,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="130" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B130" s="56" t="s">
         <v>758</v>
       </c>
@@ -12922,7 +12920,7 @@
         <v>762</v>
       </c>
     </row>
-    <row r="131" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B131" s="56" t="s">
         <v>763</v>
       </c>
@@ -12981,7 +12979,7 @@
         <v>757</v>
       </c>
     </row>
-    <row r="132" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B132" s="56" t="s">
         <v>766</v>
       </c>
@@ -13040,7 +13038,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="133" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B133" s="56" t="s">
         <v>898</v>
       </c>
@@ -13099,7 +13097,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="134" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B134" s="56" t="s">
         <v>899</v>
       </c>
@@ -13158,7 +13156,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="135" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B135" s="56" t="s">
         <v>900</v>
       </c>
@@ -13217,7 +13215,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="136" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B136" s="56" t="s">
         <v>901</v>
       </c>
@@ -13270,7 +13268,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="137" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B137" s="56" t="s">
         <v>902</v>
       </c>
@@ -13323,7 +13321,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="138" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B138" s="56" t="s">
         <v>771</v>
       </c>
@@ -13382,7 +13380,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="139" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B139" s="56" t="s">
         <v>890</v>
       </c>
@@ -13441,7 +13439,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="140" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B140" s="56" t="s">
         <v>891</v>
       </c>
@@ -13500,7 +13498,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="141" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B141" s="56" t="s">
         <v>892</v>
       </c>
@@ -13559,7 +13557,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="142" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B142" s="56" t="s">
         <v>893</v>
       </c>
@@ -13612,7 +13610,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="143" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B143" s="56" t="s">
         <v>894</v>
       </c>
@@ -13665,7 +13663,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="144" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B144" s="56" t="s">
         <v>774</v>
       </c>
@@ -13724,7 +13722,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="145" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B145" s="56" t="s">
         <v>776</v>
       </c>
@@ -13783,7 +13781,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="146" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B146" s="56" t="s">
         <v>779</v>
       </c>
@@ -13842,7 +13840,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="147" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B147" s="56" t="s">
         <v>783</v>
       </c>
@@ -13901,7 +13899,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="148" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B148" s="56" t="s">
         <v>786</v>
       </c>
@@ -13960,7 +13958,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="149" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B149" s="56" t="s">
         <v>788</v>
       </c>
@@ -14019,7 +14017,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="150" spans="2:26" hidden="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="2:26" x14ac:dyDescent="0.3">
       <c r="B150" s="56" t="s">
         <v>791</v>
       </c>
@@ -14248,11 +14246,6 @@
     </row>
   </sheetData>
   <autoFilter ref="B2:AA150" xr:uid="{3941833B-CC47-4797-9275-893CD4E748EC}">
-    <filterColumn colId="5">
-      <customFilters>
-        <customFilter val="PB*"/>
-      </customFilters>
-    </filterColumn>
     <filterColumn colId="18" showButton="0"/>
     <filterColumn colId="19" showButton="0"/>
     <filterColumn colId="20" showButton="0"/>
@@ -14264,6 +14257,7 @@
     <mergeCell ref="T2:W2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>